<commit_message>
bagging and sarimax model
</commit_message>
<xml_diff>
--- a/data/forecasting_data/exog_data/월_BTS콘서트.xlsx
+++ b/data/forecasting_data/exog_data/월_BTS콘서트.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\jupyter_project\demand_forecasting\demand_forecasting\data\forecasting_data\exog_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\jupyter_project\demand_forecasting\data\forecasting_data\exog_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F58B7-3C17-4592-88B3-01ABB359AA98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07ADF7B-554F-4284-911E-08E173D174A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -28,18 +23,17 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>특징값</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +42,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -72,12 +73,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -86,7 +102,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -96,7 +114,7 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -119,44 +137,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -183,15 +201,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -218,7 +235,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -230,142 +246,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -373,14 +413,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -396,7 +435,7 @@
         <v>37622</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -404,7 +443,7 @@
         <v>37653</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -412,7 +451,7 @@
         <v>37681</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -420,7 +459,7 @@
         <v>37712</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -428,7 +467,7 @@
         <v>37742</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -436,7 +475,7 @@
         <v>37773</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -444,7 +483,7 @@
         <v>37803</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -452,7 +491,7 @@
         <v>37834</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -460,7 +499,7 @@
         <v>37865</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -468,7 +507,7 @@
         <v>37895</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -476,7 +515,7 @@
         <v>37926</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -484,7 +523,7 @@
         <v>37956</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -492,7 +531,7 @@
         <v>37987</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -500,7 +539,7 @@
         <v>38018</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
@@ -508,7 +547,7 @@
         <v>38047</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
@@ -516,7 +555,7 @@
         <v>38078</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -524,7 +563,7 @@
         <v>38108</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -532,7 +571,7 @@
         <v>38139</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
@@ -540,7 +579,7 @@
         <v>38169</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
@@ -548,7 +587,7 @@
         <v>38200</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
@@ -556,7 +595,7 @@
         <v>38231</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
@@ -564,7 +603,7 @@
         <v>38261</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -572,7 +611,7 @@
         <v>38292</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -580,7 +619,7 @@
         <v>38322</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
@@ -588,7 +627,7 @@
         <v>38353</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
@@ -596,7 +635,7 @@
         <v>38384</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
@@ -604,7 +643,7 @@
         <v>38412</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -612,7 +651,7 @@
         <v>38443</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
@@ -620,7 +659,7 @@
         <v>38473</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -628,7 +667,7 @@
         <v>38504</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
@@ -636,7 +675,7 @@
         <v>38534</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
@@ -644,7 +683,7 @@
         <v>38565</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
@@ -652,7 +691,7 @@
         <v>38596</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -660,7 +699,7 @@
         <v>38626</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -668,7 +707,7 @@
         <v>38657</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -676,7 +715,7 @@
         <v>38687</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -684,7 +723,7 @@
         <v>38718</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -692,7 +731,7 @@
         <v>38749</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -700,7 +739,7 @@
         <v>38777</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -708,7 +747,7 @@
         <v>38808</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -716,7 +755,7 @@
         <v>38838</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -724,7 +763,7 @@
         <v>38869</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -732,7 +771,7 @@
         <v>38899</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
@@ -740,7 +779,7 @@
         <v>38930</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
@@ -748,7 +787,7 @@
         <v>38961</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -756,7 +795,7 @@
         <v>38991</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
@@ -764,7 +803,7 @@
         <v>39022</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -772,7 +811,7 @@
         <v>39052</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -780,7 +819,7 @@
         <v>39083</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -788,7 +827,7 @@
         <v>39114</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
@@ -796,7 +835,7 @@
         <v>39142</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -804,7 +843,7 @@
         <v>39173</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
@@ -812,7 +851,7 @@
         <v>39203</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
@@ -820,7 +859,7 @@
         <v>39234</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
@@ -828,7 +867,7 @@
         <v>39264</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
@@ -836,7 +875,7 @@
         <v>39295</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -844,7 +883,7 @@
         <v>39326</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -852,7 +891,7 @@
         <v>39356</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
@@ -860,7 +899,7 @@
         <v>39387</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
@@ -868,7 +907,7 @@
         <v>39417</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -876,7 +915,7 @@
         <v>39448</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
@@ -884,7 +923,7 @@
         <v>39479</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -892,7 +931,7 @@
         <v>39508</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
@@ -900,7 +939,7 @@
         <v>39539</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
@@ -908,7 +947,7 @@
         <v>39569</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -916,7 +955,7 @@
         <v>39600</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -924,7 +963,7 @@
         <v>39630</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
@@ -932,7 +971,7 @@
         <v>39661</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
@@ -940,7 +979,7 @@
         <v>39692</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
@@ -948,7 +987,7 @@
         <v>39722</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
@@ -956,7 +995,7 @@
         <v>39753</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
@@ -964,7 +1003,7 @@
         <v>39783</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.4">
@@ -972,7 +1011,7 @@
         <v>39814</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.4">
@@ -980,7 +1019,7 @@
         <v>39845</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
@@ -988,7 +1027,7 @@
         <v>39873</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.4">
@@ -996,7 +1035,7 @@
         <v>39904</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.4">
@@ -1004,7 +1043,7 @@
         <v>39934</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
@@ -1012,7 +1051,7 @@
         <v>39965</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.4">
@@ -1020,7 +1059,7 @@
         <v>39995</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.4">
@@ -1028,7 +1067,7 @@
         <v>40026</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.4">
@@ -1036,7 +1075,7 @@
         <v>40057</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.4">
@@ -1044,7 +1083,7 @@
         <v>40087</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.4">
@@ -1052,7 +1091,7 @@
         <v>40118</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.4">
@@ -1060,7 +1099,7 @@
         <v>40148</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.4">
@@ -1068,7 +1107,7 @@
         <v>40179</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.4">
@@ -1076,7 +1115,7 @@
         <v>40210</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.4">
@@ -1084,7 +1123,7 @@
         <v>40238</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.4">
@@ -1092,7 +1131,7 @@
         <v>40269</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.4">
@@ -1100,7 +1139,7 @@
         <v>40299</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.4">
@@ -1108,7 +1147,7 @@
         <v>40330</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.4">
@@ -1116,7 +1155,7 @@
         <v>40360</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.4">
@@ -1124,7 +1163,7 @@
         <v>40391</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.4">
@@ -1132,7 +1171,7 @@
         <v>40422</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.4">
@@ -1140,7 +1179,7 @@
         <v>40452</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.4">
@@ -1148,7 +1187,7 @@
         <v>40483</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.4">
@@ -1156,7 +1195,7 @@
         <v>40513</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.4">
@@ -1164,7 +1203,7 @@
         <v>40544</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.4">
@@ -1172,7 +1211,7 @@
         <v>40575</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.4">
@@ -1180,7 +1219,7 @@
         <v>40603</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.4">
@@ -1188,7 +1227,7 @@
         <v>40634</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.4">
@@ -1196,7 +1235,7 @@
         <v>40664</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.4">
@@ -1204,7 +1243,7 @@
         <v>40695</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.4">
@@ -1212,7 +1251,7 @@
         <v>40725</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.4">
@@ -1220,7 +1259,7 @@
         <v>40756</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.4">
@@ -1228,7 +1267,7 @@
         <v>40787</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.4">
@@ -1236,7 +1275,7 @@
         <v>40817</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.4">
@@ -1244,7 +1283,7 @@
         <v>40848</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.4">
@@ -1252,7 +1291,7 @@
         <v>40878</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.4">
@@ -1260,7 +1299,7 @@
         <v>40909</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.4">
@@ -1268,7 +1307,7 @@
         <v>40940</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.4">
@@ -1276,7 +1315,7 @@
         <v>40969</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.4">
@@ -1284,7 +1323,7 @@
         <v>41000</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.4">
@@ -1292,7 +1331,7 @@
         <v>41030</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.4">
@@ -1300,7 +1339,7 @@
         <v>41061</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.4">
@@ -1308,7 +1347,7 @@
         <v>41091</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.4">
@@ -1316,7 +1355,7 @@
         <v>41122</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.4">
@@ -1324,7 +1363,7 @@
         <v>41153</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.4">
@@ -1332,7 +1371,7 @@
         <v>41183</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.4">
@@ -1340,7 +1379,7 @@
         <v>41214</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.4">
@@ -1348,7 +1387,7 @@
         <v>41244</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.4">
@@ -1356,7 +1395,7 @@
         <v>41275</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.4">
@@ -1364,7 +1403,7 @@
         <v>41306</v>
       </c>
       <c r="B123">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.4">
@@ -1372,7 +1411,7 @@
         <v>41334</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.4">
@@ -1380,7 +1419,7 @@
         <v>41365</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.4">
@@ -1388,7 +1427,7 @@
         <v>41395</v>
       </c>
       <c r="B126">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.4">
@@ -1396,7 +1435,7 @@
         <v>41426</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.4">
@@ -1404,7 +1443,7 @@
         <v>41456</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.4">
@@ -1412,7 +1451,7 @@
         <v>41487</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.4">
@@ -1420,7 +1459,7 @@
         <v>41518</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.4">
@@ -1428,7 +1467,7 @@
         <v>41548</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.4">
@@ -1436,7 +1475,7 @@
         <v>41579</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.4">
@@ -1444,7 +1483,7 @@
         <v>41609</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.4">
@@ -1452,7 +1491,7 @@
         <v>41640</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.4">
@@ -1460,7 +1499,7 @@
         <v>41671</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.4">
@@ -1468,7 +1507,7 @@
         <v>41699</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.4">
@@ -1476,7 +1515,7 @@
         <v>41730</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.4">
@@ -1484,7 +1523,7 @@
         <v>41760</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.4">
@@ -1492,7 +1531,7 @@
         <v>41791</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.4">
@@ -1500,7 +1539,7 @@
         <v>41821</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.4">
@@ -1508,7 +1547,7 @@
         <v>41852</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.4">
@@ -1516,7 +1555,7 @@
         <v>41883</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.4">
@@ -1524,7 +1563,7 @@
         <v>41913</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.4">
@@ -1532,7 +1571,7 @@
         <v>41944</v>
       </c>
       <c r="B144">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.4">
@@ -1540,7 +1579,7 @@
         <v>41974</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>0.21428571428571441</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.4">
@@ -1548,7 +1587,7 @@
         <v>42005</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>0.57142857142857162</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.4">
@@ -1556,7 +1595,7 @@
         <v>42036</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>0.57142857142857162</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.4">
@@ -1564,7 +1603,7 @@
         <v>42064</v>
       </c>
       <c r="B148">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.4">
@@ -1572,7 +1611,7 @@
         <v>42095</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.4">
@@ -1580,7 +1619,7 @@
         <v>42125</v>
       </c>
       <c r="B150">
-        <v>0</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.4">
@@ -1588,7 +1627,7 @@
         <v>42156</v>
       </c>
       <c r="B151">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.4">
@@ -1596,7 +1635,7 @@
         <v>42186</v>
       </c>
       <c r="B152">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.4">
@@ -1604,7 +1643,7 @@
         <v>42217</v>
       </c>
       <c r="B153">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.4">
@@ -1612,7 +1651,7 @@
         <v>42248</v>
       </c>
       <c r="B154">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.4">
@@ -1620,7 +1659,7 @@
         <v>42278</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.4">
@@ -1628,7 +1667,7 @@
         <v>42309</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.4">
@@ -1636,7 +1675,7 @@
         <v>42339</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.4">
@@ -1644,7 +1683,7 @@
         <v>42370</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.4">
@@ -1652,7 +1691,7 @@
         <v>42401</v>
       </c>
       <c r="B159">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.4">
@@ -1660,7 +1699,7 @@
         <v>42430</v>
       </c>
       <c r="B160">
-        <v>2</v>
+        <v>7.1428571428571563E-2</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.4">
@@ -1676,7 +1715,7 @@
         <v>42491</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.4">
@@ -1684,7 +1723,7 @@
         <v>42522</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.4">
@@ -1692,7 +1731,7 @@
         <v>42552</v>
       </c>
       <c r="B164">
-        <v>2</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.4">
@@ -1700,7 +1739,7 @@
         <v>42583</v>
       </c>
       <c r="B165">
-        <v>2</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.4">
@@ -1708,7 +1747,7 @@
         <v>42614</v>
       </c>
       <c r="B166">
-        <v>0</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.4">
@@ -1716,7 +1755,7 @@
         <v>42644</v>
       </c>
       <c r="B167">
-        <v>0</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.4">
@@ -1724,7 +1763,7 @@
         <v>42675</v>
       </c>
       <c r="B168">
-        <v>0</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.4">
@@ -1732,7 +1771,7 @@
         <v>42705</v>
       </c>
       <c r="B169">
-        <v>0</v>
+        <v>0.35714285714285732</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.4">
@@ -1740,7 +1779,7 @@
         <v>42736</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>0.66071428571428581</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.4">
@@ -1748,7 +1787,7 @@
         <v>42767</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>0.64285714285714302</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.4">
@@ -1756,7 +1795,7 @@
         <v>42795</v>
       </c>
       <c r="B172">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.4">
@@ -1764,7 +1803,7 @@
         <v>42826</v>
       </c>
       <c r="B173">
-        <v>2</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.4">
@@ -1772,7 +1811,7 @@
         <v>42856</v>
       </c>
       <c r="B174">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.4">
@@ -1780,7 +1819,7 @@
         <v>42887</v>
       </c>
       <c r="B175">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.4">
@@ -1788,7 +1827,7 @@
         <v>42917</v>
       </c>
       <c r="B176">
-        <v>2</v>
+        <v>0.14285714285714299</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.4">
@@ -1796,7 +1835,7 @@
         <v>42948</v>
       </c>
       <c r="B177">
-        <v>0</v>
+        <v>0.14285714285714299</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.4">
@@ -1804,7 +1843,7 @@
         <v>42979</v>
       </c>
       <c r="B178">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.4">
@@ -1812,7 +1851,7 @@
         <v>43009</v>
       </c>
       <c r="B179">
-        <v>2</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.4">
@@ -1820,7 +1859,7 @@
         <v>43040</v>
       </c>
       <c r="B180">
-        <v>2</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.4">
@@ -1828,7 +1867,7 @@
         <v>43070</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.4">
@@ -1836,7 +1875,7 @@
         <v>43101</v>
       </c>
       <c r="B182">
-        <v>0</v>
+        <v>0.28571428571428592</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.4">
@@ -1844,7 +1883,7 @@
         <v>43132</v>
       </c>
       <c r="B183">
-        <v>0</v>
+        <v>0.57142857142857162</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.4">
@@ -1852,7 +1891,7 @@
         <v>43160</v>
       </c>
       <c r="B184">
-        <v>0</v>
+        <v>0.85714285714285743</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.4">
@@ -1860,7 +1899,7 @@
         <v>43191</v>
       </c>
       <c r="B185">
-        <v>0</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.4">
@@ -1868,7 +1907,7 @@
         <v>43221</v>
       </c>
       <c r="B186">
-        <v>0</v>
+        <v>0.50000000000000011</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.4">
@@ -1876,7 +1915,7 @@
         <v>43252</v>
       </c>
       <c r="B187">
-        <v>0</v>
+        <v>0.17857142857142869</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.4">
@@ -1884,7 +1923,7 @@
         <v>43282</v>
       </c>
       <c r="B188">
-        <v>0</v>
+        <v>0.57142857142857162</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.4">
@@ -1892,7 +1931,7 @@
         <v>43313</v>
       </c>
       <c r="B189">
-        <v>1</v>
+        <v>0.35714285714285732</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.4">
@@ -1900,7 +1939,7 @@
         <v>43344</v>
       </c>
       <c r="B190">
-        <v>2</v>
+        <v>0.28571428571428592</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.4">
@@ -1908,7 +1947,7 @@
         <v>43374</v>
       </c>
       <c r="B191">
-        <v>2</v>
+        <v>0.28571428571428592</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.4">
@@ -1916,7 +1955,7 @@
         <v>43405</v>
       </c>
       <c r="B192">
-        <v>2</v>
+        <v>0.23214285714285729</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.4">
@@ -1924,7 +1963,7 @@
         <v>43435</v>
       </c>
       <c r="B193">
-        <v>0</v>
+        <v>0.50000000000000011</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.4">
@@ -1932,7 +1971,7 @@
         <v>43466</v>
       </c>
       <c r="B194">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.4">
@@ -1940,7 +1979,7 @@
         <v>43497</v>
       </c>
       <c r="B195">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.4">
@@ -1948,7 +1987,7 @@
         <v>43525</v>
       </c>
       <c r="B196">
-        <v>2</v>
+        <v>0.71428571428571441</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.4">
@@ -1956,7 +1995,7 @@
         <v>43556</v>
       </c>
       <c r="B197">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.4">
@@ -1964,7 +2003,7 @@
         <v>43586</v>
       </c>
       <c r="B198">
-        <v>2</v>
+        <v>0.14285714285714299</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.4">
@@ -1972,7 +2011,7 @@
         <v>43617</v>
       </c>
       <c r="B199">
-        <v>2</v>
+        <v>0.14285714285714299</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.4">
@@ -1980,7 +2019,7 @@
         <v>43647</v>
       </c>
       <c r="B200">
-        <v>2</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.4">
@@ -1988,7 +2027,7 @@
         <v>43678</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.4">
@@ -1996,7 +2035,7 @@
         <v>43709</v>
       </c>
       <c r="B202">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.4">
@@ -2004,7 +2043,7 @@
         <v>43739</v>
       </c>
       <c r="B203">
-        <v>1</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.4">
@@ -2012,7 +2051,7 @@
         <v>43770</v>
       </c>
       <c r="B204">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.4">
@@ -2020,7 +2059,7 @@
         <v>43800</v>
       </c>
       <c r="B205">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.4">
@@ -2028,7 +2067,7 @@
         <v>43831</v>
       </c>
       <c r="B206">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.4">
@@ -2036,7 +2075,7 @@
         <v>43862</v>
       </c>
       <c r="B207">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.4">
@@ -2044,7 +2083,7 @@
         <v>43891</v>
       </c>
       <c r="B208">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.4">
@@ -2052,7 +2091,7 @@
         <v>43922</v>
       </c>
       <c r="B209">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.4">
@@ -2060,7 +2099,7 @@
         <v>43952</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.4">
@@ -2068,7 +2107,7 @@
         <v>43983</v>
       </c>
       <c r="B211">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.4">
@@ -2076,7 +2115,7 @@
         <v>44013</v>
       </c>
       <c r="B212">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.4">
@@ -2084,7 +2123,7 @@
         <v>44044</v>
       </c>
       <c r="B213">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.4">
@@ -2092,7 +2131,7 @@
         <v>44075</v>
       </c>
       <c r="B214">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.4">
@@ -2100,7 +2139,7 @@
         <v>44105</v>
       </c>
       <c r="B215">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.4">
@@ -2108,7 +2147,7 @@
         <v>44136</v>
       </c>
       <c r="B216">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.4">
@@ -2116,12 +2155,12 @@
         <v>44166</v>
       </c>
       <c r="B217">
-        <v>0</v>
+        <v>0.42857142857142871</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>